<commit_message>
added updated Final Release
</commit_message>
<xml_diff>
--- a/Final Release/FinalRelease_TestReport.xlsx
+++ b/Final Release/FinalRelease_TestReport.xlsx
@@ -5,10 +5,10 @@
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fabian\nani\Unit13_Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fabian\nani\project-proposal-die_gottlichen_socken\Final Release\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F59A5AC-D488-4B1C-84E0-305DDD92FDE1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFBB9F1E-D1FC-4A6C-83D6-0CE9DF34248F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -387,7 +387,22 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -506,7 +521,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -622,9 +652,24 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1958,7 +2003,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2004,64 +2049,114 @@
         <v>0</v>
       </c>
       <c r="D3" s="4">
-        <f t="shared" ref="D3:D22" si="0">E3-C3-B3</f>
-        <v>16</v>
+        <f t="shared" ref="D3" si="0">E3-C3-B3</f>
+        <v>21</v>
       </c>
       <c r="E3" s="4">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>6</v>
+      <c r="A4" s="5">
+        <v>42144</v>
       </c>
       <c r="B4" s="6">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C4" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D4" s="6">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E4" s="6">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
+      <c r="A5" s="5">
+        <v>42151</v>
+      </c>
+      <c r="B5" s="6">
+        <v>20</v>
+      </c>
+      <c r="C5" s="6">
+        <v>5</v>
+      </c>
+      <c r="D5" s="6">
+        <v>10</v>
+      </c>
+      <c r="E5" s="6">
+        <v>35</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
+      <c r="A6" s="5">
+        <v>42158</v>
+      </c>
+      <c r="B6" s="6">
+        <v>24</v>
+      </c>
+      <c r="C6" s="6">
+        <v>9</v>
+      </c>
+      <c r="D6" s="6">
+        <v>2</v>
+      </c>
+      <c r="E6" s="6">
+        <v>35</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+      <c r="A7" s="5">
+        <v>42165</v>
+      </c>
+      <c r="B7" s="6">
+        <v>28</v>
+      </c>
+      <c r="C7" s="6">
+        <v>6</v>
+      </c>
+      <c r="D7" s="6">
+        <v>1</v>
+      </c>
+      <c r="E7" s="6">
+        <v>35</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="A8" s="5">
+        <v>42172</v>
+      </c>
+      <c r="B8" s="6">
+        <v>30</v>
+      </c>
+      <c r="C8" s="6">
+        <v>5</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0</v>
+      </c>
+      <c r="E8" s="6">
+        <v>35</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
+      <c r="A9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="6">
+        <v>31</v>
+      </c>
+      <c r="C9" s="6">
+        <v>4</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0</v>
+      </c>
+      <c r="E9" s="6">
+        <v>35</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>

</xml_diff>